<commit_message>
First version of Insights AI
</commit_message>
<xml_diff>
--- a/uploads/acidentesJan2024_todas_causas_tipos_ex.xlsx
+++ b/uploads/acidentesJan2024_todas_causas_tipos_ex.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gadm1\Desktop\Projetos\AI-simple-app\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gadm1\Desktop\TABELAS PARA TESTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3AF526-706E-4EF4-829F-6F7D6E216D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A5F38CD-36F6-4951-AF7F-384942B50F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1DBEAE3A-AEC5-4DFA-8A09-A180915D881F}"/>
   </bookViews>
@@ -1218,9 +1218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FBE4D0-E73F-481E-A347-DA7CCFAFB70E}">
   <dimension ref="A1:AK25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AB27" sqref="AB27"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1228,7 +1226,6 @@
     <col min="9" max="9" width="14.6640625" customWidth="1"/>
     <col min="11" max="11" width="18.88671875" customWidth="1"/>
     <col min="22" max="22" width="19.6640625" customWidth="1"/>
-    <col min="28" max="28" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.3">
@@ -1653,7 +1650,7 @@
         <v>61</v>
       </c>
       <c r="AB4" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="AC4" t="s">
         <v>61</v>
@@ -1992,7 +1989,7 @@
         <v>61</v>
       </c>
       <c r="AB7" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="AC7" t="s">
         <v>61</v>
@@ -2331,7 +2328,7 @@
         <v>61</v>
       </c>
       <c r="AB10" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="AC10" t="s">
         <v>61</v>
@@ -4026,7 +4023,7 @@
         <v>61</v>
       </c>
       <c r="AB25" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="AC25">
         <v>0</v>

</xml_diff>